<commit_message>
Updated the NewChoiceCard Template. Added some new cards: Implemented custom Fatal Effect in Purge the Sinful Created LightDark Power (names not flavoured yet)
Implemented UI for Soul Health (this is HUGE) complete with "second healthbar" colored and text.
Still need to implement soul health functionality, but that should be trivial now that I know how to use the power of spirepatches and all that java assist injection stuff :D
</commit_message>
<xml_diff>
--- a/Basegame Character Card Stats.xlsx
+++ b/Basegame Character Card Stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20339"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Stuff\Coding\ModdingSlayTheSpire\my_mods\git\StS-DefaultModBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zacc\Documents\StS Modding\StS-DefaultModBase-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4D4958-2D4A-4279-92AE-904F3C9F1E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B433FC-F9C0-45D4-8D43-828BE3332BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="278" xr2:uid="{AD2E1A73-3376-4E41-A344-6779F4DBBFBB}"/>
+    <workbookView xWindow="4830" yWindow="2400" windowWidth="17220" windowHeight="9720" tabRatio="278" xr2:uid="{AD2E1A73-3376-4E41-A344-6779F4DBBFBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -237,6 +245,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -244,15 +261,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -265,6 +273,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -288,15 +299,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -325,6 +327,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -344,15 +361,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -387,6 +395,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -406,21 +423,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -437,6 +439,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -515,17 +523,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Cost" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Cost" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="F6:I10" xr:uid="{CE12703D-A0E8-4EAA-9688-E5928D5B5BFB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -533,23 +541,23 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Rarity" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Rarity" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FEC834A-9605-4DAB-8FC8-559DFE95E7CE}" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FEC834A-9605-4DAB-8FC8-559DFE95E7CE}" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="F16:I19" xr:uid="{AB9EBA6F-19E5-4878-B4BF-640070BDE1CB}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{10488BD1-9981-44C8-B679-8617EA80CFDF}" name="Type" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2BD6E313-819A-4120-B615-A73747A8BFF9}" name="Silent" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{29092D1A-1D35-4F6E-9938-E644E403DC81}" name="Ironclad" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D8133038-6E03-4174-95AC-6C4D249B7298}" name="Defect" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{10488BD1-9981-44C8-B679-8617EA80CFDF}" name="Type" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2BD6E313-819A-4120-B615-A73747A8BFF9}" name="Silent" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{29092D1A-1D35-4F6E-9938-E644E403DC81}" name="Ironclad" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D8133038-6E03-4174-95AC-6C4D249B7298}" name="Defect" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -855,7 +863,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,47 +872,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="F5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1097,24 +1105,24 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="9" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
       <c r="F16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1129,11 +1137,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="F17" s="12" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="F17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="4">
@@ -1149,7 +1157,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="4">
@@ -1165,7 +1173,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="4">

</xml_diff>